<commit_message>
HoloLens QoE User Study
</commit_message>
<xml_diff>
--- a/HoloLens QoE User Study Results.xlsx
+++ b/HoloLens QoE User Study Results.xlsx
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Q14</t>
-  </si>
-  <si>
-    <t>Q15</t>
   </si>
   <si>
     <t>Rating</t>
@@ -163,6 +160,9 @@
       </rPr>
       <t>f</t>
     </r>
+  </si>
+  <si>
+    <t>Q6</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD49" sqref="AD49:AD63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF72" sqref="AF72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -581,7 +581,7 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
@@ -589,7 +589,7 @@
     </row>
     <row r="3" spans="1:33" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -619,10 +619,10 @@
         <v>8</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>9</v>
@@ -631,55 +631,55 @@
         <v>10</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="X3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC3" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="AD3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
@@ -695,13 +695,13 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>11</v>
@@ -794,13 +794,13 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3">
         <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
         <v>11</v>
@@ -893,13 +893,13 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3">
         <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -986,19 +986,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1091,13 +1091,13 @@
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E8" s="3">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1190,13 +1190,13 @@
         <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="3">
         <v>11</v>
@@ -1283,19 +1283,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3">
         <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3">
         <v>11</v>
@@ -1382,19 +1382,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3">
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3">
         <v>11</v>
@@ -1487,13 +1487,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="3">
         <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1586,13 +1586,13 @@
         <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1685,13 +1685,13 @@
         <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="3">
         <v>11</v>
@@ -1784,13 +1784,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="3">
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1883,13 +1883,13 @@
         <v>20</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="3">
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="3">
         <v>11</v>
@@ -1976,19 +1976,19 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3">
         <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3">
         <v>11</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -2075,19 +2075,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>30</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="3">
         <v>5</v>
@@ -2180,13 +2180,13 @@
         <v>30</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3">
         <v>11</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -2273,19 +2273,19 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3">
         <v>30</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -2372,19 +2372,19 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="3">
         <v>30</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3">
         <v>11</v>
@@ -2477,13 +2477,13 @@
         <v>30</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3">
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="3">
         <v>5</v>
@@ -2570,19 +2570,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3">
         <v>20</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="3">
         <v>11</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="3">
         <v>1</v>
@@ -2675,13 +2675,13 @@
         <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -2774,13 +2774,13 @@
         <v>30</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E25" s="3">
         <v>11</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" s="3">
         <v>11</v>
@@ -2873,13 +2873,13 @@
         <v>20</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E26" s="3">
         <v>11</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="3">
         <v>1</v>
@@ -2966,19 +2966,19 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="3">
         <v>20</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27" s="3">
         <v>1</v>
@@ -3071,13 +3071,13 @@
         <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="3">
         <v>11</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G28" s="3">
         <v>1</v>
@@ -3170,13 +3170,13 @@
         <v>10</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="3">
         <v>1</v>
@@ -3269,13 +3269,13 @@
         <v>40</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="3">
         <v>0</v>
@@ -3362,19 +3362,19 @@
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="3">
         <v>30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="3">
         <v>1</v>
@@ -3455,7 +3455,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
@@ -3469,13 +3469,13 @@
         <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="3">
         <v>1</v>
@@ -3562,19 +3562,19 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="3">
         <v>30</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G33" s="3">
         <v>11</v>
@@ -3661,19 +3661,19 @@
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="3">
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G34" s="3">
         <v>1</v>
@@ -3760,19 +3760,19 @@
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="3">
         <v>30</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -3865,13 +3865,13 @@
         <v>30</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="3">
+        <v>5</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E36" s="3">
-        <v>5</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
@@ -3889,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="L36" s="4">
-        <f t="shared" ref="L36:L67" si="4">(K36-1)/4*100</f>
+        <f t="shared" ref="L36:L63" si="4">(K36-1)/4*100</f>
         <v>75</v>
       </c>
       <c r="M36" s="3">
@@ -3902,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="P36" s="4">
-        <f t="shared" ref="P36:P67" si="5">(O36-1)/4*100</f>
+        <f t="shared" ref="P36:P63" si="5">(O36-1)/4*100</f>
         <v>75</v>
       </c>
       <c r="Q36" s="3">
@@ -3921,7 +3921,7 @@
         <v>3</v>
       </c>
       <c r="V36" s="4">
-        <f t="shared" ref="V36:V67" si="6">(U36-1)/4*100</f>
+        <f t="shared" ref="V36:V63" si="6">(U36-1)/4*100</f>
         <v>50</v>
       </c>
       <c r="W36" s="3">
@@ -3943,7 +3943,7 @@
         <v>3</v>
       </c>
       <c r="AC36" s="4">
-        <f t="shared" ref="AC36:AC67" si="7">(AB36-1)/4*100</f>
+        <f t="shared" ref="AC36:AC63" si="7">(AB36-1)/4*100</f>
         <v>50</v>
       </c>
       <c r="AD36" s="3">
@@ -3958,19 +3958,19 @@
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="3">
         <v>20</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37" s="3">
         <v>0</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G37" s="3">
         <v>0</v>
@@ -4063,13 +4063,13 @@
         <v>20</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E38" s="3">
         <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38" s="3">
         <v>5</v>
@@ -4156,19 +4156,19 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C39" s="3">
         <v>20</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="3">
         <v>1</v>
@@ -4255,19 +4255,19 @@
         <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C40" s="3">
         <v>20</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G40" s="3">
         <v>0</v>
@@ -4354,19 +4354,19 @@
         <v>38</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C41" s="3">
         <v>20</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G41" s="3">
         <v>0</v>
@@ -4459,13 +4459,13 @@
         <v>20</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" s="3">
         <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G42" s="3">
         <v>5</v>
@@ -4558,13 +4558,13 @@
         <v>20</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G43" s="3">
         <v>11</v>
@@ -4651,19 +4651,19 @@
         <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" s="3">
         <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E44" s="3">
         <v>11</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
@@ -4756,13 +4756,13 @@
         <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E45" s="3">
         <v>11</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G45" s="3">
         <v>11</v>
@@ -4855,13 +4855,13 @@
         <v>30</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G46" s="3">
         <v>11</v>
@@ -4954,13 +4954,13 @@
         <v>20</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G47" s="3">
         <v>1</v>
@@ -5053,13 +5053,13 @@
         <v>20</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G48" s="3">
         <v>11</v>
@@ -5152,13 +5152,13 @@
         <v>20</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E49" s="3">
         <v>11</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G49" s="3">
         <v>11</v>
@@ -5247,19 +5247,19 @@
         <v>47</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="3">
         <v>20</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G50" s="3">
         <v>0</v>
@@ -5354,13 +5354,13 @@
         <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G51" s="3">
         <v>1</v>
@@ -5455,13 +5455,13 @@
         <v>10</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E52" s="3">
         <v>0</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G52" s="3">
         <v>1</v>
@@ -5550,19 +5550,19 @@
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53" s="3">
         <v>20</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G53" s="3">
         <v>1</v>
@@ -5657,13 +5657,13 @@
         <v>20</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E54" s="3">
         <v>11</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G54" s="3">
         <v>5</v>
@@ -5752,19 +5752,19 @@
         <v>52</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="3">
         <v>20</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E55" s="3">
         <v>0</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G55" s="3">
         <v>0</v>
@@ -5859,13 +5859,13 @@
         <v>20</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E56" s="3">
         <v>11</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G56" s="3">
         <v>11</v>
@@ -5960,13 +5960,13 @@
         <v>20</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E57" s="3">
-        <v>1</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G57" s="3">
         <v>0</v>
@@ -6061,13 +6061,13 @@
         <v>10</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" s="3">
         <v>11</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G58" s="3">
         <v>5</v>
@@ -6156,19 +6156,19 @@
         <v>56</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C59" s="3">
         <v>20</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59" s="3">
         <v>0</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G59" s="3">
         <v>11</v>
@@ -6257,19 +6257,19 @@
         <v>57</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60" s="3">
         <v>10</v>
       </c>
       <c r="D60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="3">
+        <v>5</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E60" s="3">
-        <v>5</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G60" s="3">
         <v>0</v>
@@ -6364,13 +6364,13 @@
         <v>40</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E61" s="3">
         <v>0</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G61" s="3">
         <v>0</v>
@@ -6465,13 +6465,13 @@
         <v>30</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E62" s="3">
         <v>0</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G62" s="3">
         <v>11</v>
@@ -6560,19 +6560,19 @@
         <v>60</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C63" s="3">
         <v>20</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G63" s="3">
         <v>0</v>
@@ -6668,12 +6668,12 @@
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
@@ -6703,10 +6703,10 @@
         <v>8</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M68" t="s">
         <v>9</v>
@@ -6715,55 +6715,55 @@
         <v>10</v>
       </c>
       <c r="O68" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T68" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U68" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P68" s="4" t="s">
+      <c r="V68" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q68" t="s">
-        <v>11</v>
-      </c>
-      <c r="R68" t="s">
-        <v>12</v>
-      </c>
-      <c r="S68" t="s">
-        <v>13</v>
-      </c>
-      <c r="T68" t="s">
+      <c r="W68" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U68" s="2" t="s">
+      <c r="X68" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z68" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB68" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V68" s="4" t="s">
+      <c r="AC68" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="W68" t="s">
-        <v>15</v>
-      </c>
-      <c r="X68" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA68" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB68" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC68" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="AD68" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE68" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="AE68" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="AF68" s="4"/>
     </row>
@@ -6778,13 +6778,13 @@
         <v>20</v>
       </c>
       <c r="D69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E69">
         <v>11</v>
       </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G69">
         <v>11</v>
@@ -6859,7 +6859,7 @@
         <f t="shared" ref="AC69:AC83" si="10">(AB69-1)/4*100</f>
         <v>75</v>
       </c>
-      <c r="AD69">
+      <c r="AD69" s="7">
         <v>90</v>
       </c>
       <c r="AE69" s="5">
@@ -6877,13 +6877,13 @@
         <v>20</v>
       </c>
       <c r="D70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E70">
         <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G70">
         <v>11</v>
@@ -6958,7 +6958,7 @@
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="AD70">
+      <c r="AD70" s="7">
         <v>92</v>
       </c>
       <c r="AE70" s="5">
@@ -6976,13 +6976,13 @@
         <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G71">
         <v>1</v>
@@ -7057,7 +7057,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD71">
+      <c r="AD71" s="7">
         <v>90</v>
       </c>
       <c r="AE71" s="5">
@@ -7075,13 +7075,13 @@
         <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E72">
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -7156,7 +7156,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD72">
+      <c r="AD72" s="7">
         <v>95</v>
       </c>
       <c r="AE72" s="5">
@@ -7174,13 +7174,13 @@
         <v>40</v>
       </c>
       <c r="D73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -7255,7 +7255,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD73">
+      <c r="AD73" s="7">
         <v>75</v>
       </c>
       <c r="AE73" s="5">
@@ -7273,13 +7273,13 @@
         <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E74">
         <v>11</v>
       </c>
       <c r="F74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G74">
         <v>6</v>
@@ -7354,7 +7354,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD74">
+      <c r="AD74" s="7">
         <v>80</v>
       </c>
       <c r="AE74" s="5">
@@ -7372,13 +7372,13 @@
         <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E75">
         <v>6</v>
       </c>
       <c r="F75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -7453,7 +7453,7 @@
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="AD75">
+      <c r="AD75" s="7">
         <v>90</v>
       </c>
       <c r="AE75" s="5">
@@ -7471,13 +7471,13 @@
         <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -7552,7 +7552,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD76">
+      <c r="AD76" s="7">
         <v>80</v>
       </c>
       <c r="AE76" s="5">
@@ -7564,19 +7564,19 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C77">
         <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -7651,7 +7651,7 @@
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="AD77">
+      <c r="AD77" s="7">
         <v>80</v>
       </c>
       <c r="AE77" s="5">
@@ -7663,19 +7663,19 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C78">
         <v>20</v>
       </c>
       <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
         <v>21</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78" t="s">
-        <v>22</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -7750,7 +7750,7 @@
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="AD78">
+      <c r="AD78" s="7">
         <v>98</v>
       </c>
       <c r="AE78" s="5">
@@ -7762,19 +7762,19 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C79">
         <v>30</v>
       </c>
       <c r="D79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -7849,7 +7849,7 @@
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="AD79">
+      <c r="AD79" s="7">
         <v>98</v>
       </c>
       <c r="AE79" s="5">
@@ -7867,13 +7867,13 @@
         <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E80">
         <v>11</v>
       </c>
       <c r="F80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -7948,7 +7948,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD80">
+      <c r="AD80" s="7">
         <v>70</v>
       </c>
       <c r="AE80" s="5">
@@ -7966,13 +7966,13 @@
         <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -8047,7 +8047,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD81">
+      <c r="AD81" s="7">
         <v>85</v>
       </c>
       <c r="AE81" s="5">
@@ -8065,13 +8065,13 @@
         <v>20</v>
       </c>
       <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" t="s">
         <v>21</v>
-      </c>
-      <c r="E82">
-        <v>1</v>
-      </c>
-      <c r="F82" t="s">
-        <v>22</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -8146,7 +8146,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD82">
+      <c r="AD82" s="7">
         <v>90</v>
       </c>
       <c r="AE82" s="5">
@@ -8158,19 +8158,19 @@
         <v>15</v>
       </c>
       <c r="B83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C83">
         <v>20</v>
       </c>
       <c r="D83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -8245,7 +8245,7 @@
         <f t="shared" si="10"/>
         <v>75</v>
       </c>
-      <c r="AD83">
+      <c r="AD83" s="7">
         <v>90</v>
       </c>
       <c r="AE83" s="5">

</xml_diff>